<commit_message>
redid anovas for 2019 no. of ramets
</commit_message>
<xml_diff>
--- a/2020_Relationships.xlsx
+++ b/2020_Relationships.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C71D48-A2CF-4E9C-835B-4FE71F732FC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DB21A0-1FA6-42AA-9AB9-C29E39544D4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="288" windowWidth="13680" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2019" sheetId="2" r:id="rId1"/>
+    <sheet name="2020" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
   <si>
     <t>Trait</t>
   </si>
@@ -325,18 +326,6 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -362,11 +351,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -393,6 +394,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,11 +679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CC0824-6C89-45DB-BF49-BAE4F700E378}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,227 +696,354 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E9">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="16"/>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -917,11 +1052,11 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:E15">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",B4)))</formula>
-    </cfRule>
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished integrating 2019 data with 2020 data for both stats and figures
</commit_message>
<xml_diff>
--- a/2020_Relationships.xlsx
+++ b/2020_Relationships.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DB21A0-1FA6-42AA-9AB9-C29E39544D4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E23255-CAAC-48BC-AFC4-82F9820DB3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4164" yWindow="4416" windowWidth="13680" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
     <sheet name="2020" sheetId="1" r:id="rId2"/>
+    <sheet name="Both years" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="33">
   <si>
     <t>Trait</t>
   </si>
@@ -89,13 +90,49 @@
   </si>
   <si>
     <t>Survival</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>transect, interaxn marg sig</t>
+  </si>
+  <si>
+    <t>marg sig for distance</t>
+  </si>
+  <si>
+    <t>Interaxn sig</t>
+  </si>
+  <si>
+    <t>Num. of Ramets: Mid-June</t>
+  </si>
+  <si>
+    <t>transect marg sig</t>
+  </si>
+  <si>
+    <t>transect sig</t>
+  </si>
+  <si>
+    <t>Height: Mid-June</t>
+  </si>
+  <si>
+    <t>Height: Early June</t>
+  </si>
+  <si>
+    <t>Num. of Ramets: Early June</t>
+  </si>
+  <si>
+    <t>interaxn sig when crossed (vs nested); when nested, marg sig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +162,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -323,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,23 +402,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="37">
     <dxf>
       <font>
         <b/>
@@ -376,6 +439,297 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -680,36 +1034,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CC0824-6C89-45DB-BF49-BAE4F700E378}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -725,66 +1079,156 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="B11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -792,12 +1236,108 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:E9">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="N">
+  <conditionalFormatting sqref="B3:C4">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:C5">
+    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:E5">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:C7">
+    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:C6">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:E6">
+    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:C10">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:E10">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",D10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:C11">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -810,33 +1350,33 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -865,16 +1405,16 @@
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -882,16 +1422,16 @@
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -899,16 +1439,16 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -916,16 +1456,16 @@
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -933,16 +1473,16 @@
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -950,16 +1490,16 @@
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="B9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -967,16 +1507,16 @@
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -984,16 +1524,16 @@
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="B11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1001,16 +1541,16 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="C12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1018,16 +1558,16 @@
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="B13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1051,15 +1591,193 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:E15">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
+  <conditionalFormatting sqref="B4:E6 B13:E15 B12:C12 E12 B11:D11 B10:E10 B7:C9 E7:E9">
+    <cfRule type="containsText" dxfId="16" priority="1" stopIfTrue="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA7BE2A-D5EA-475A-AE19-10551A6BB963}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14"/>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:C3 B4:E4 B8:E8 B5 D5:E5 B9:C9 E9 B6:C7">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed all ramet count models to glmer w/poisson because it's count data, not lmer.
</commit_message>
<xml_diff>
--- a/2020_Relationships.xlsx
+++ b/2020_Relationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E23255-CAAC-48BC-AFC4-82F9820DB3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A73829B-5355-4C39-A4CB-DE9613478286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4164" yWindow="4416" windowWidth="13680" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="34">
   <si>
     <t>Trait</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>interaxn sig when crossed (vs nested); when nested, marg sig</t>
+  </si>
+  <si>
+    <t>UPDATE w/glmer</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -402,6 +411,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,23 +435,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="29">
     <dxf>
       <font>
         <b/>
@@ -450,6 +460,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -576,13 +593,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -662,74 +672,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1034,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CC0824-6C89-45DB-BF49-BAE4F700E378}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,23 +989,24 @@
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="18"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1087,14 +1030,14 @@
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1104,14 +1047,14 @@
       <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1128,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1155,14 +1098,14 @@
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1172,14 +1115,17 @@
       <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F8" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1189,14 +1135,15 @@
       <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1212,8 +1159,9 @@
       <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1223,7 +1171,7 @@
       <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -1285,58 +1233,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:E10">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1363,20 +1311,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1405,16 +1353,16 @@
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1422,16 +1370,16 @@
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1439,16 +1387,16 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="B6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1456,16 +1404,16 @@
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="B7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1473,16 +1421,16 @@
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1490,16 +1438,16 @@
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="B9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1507,16 +1455,16 @@
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="18" t="s">
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1524,16 +1472,16 @@
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="B11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1541,16 +1489,16 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1558,16 +1506,16 @@
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="B13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1592,7 +1540,7 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:E6 B13:E15 B12:C12 E12 B11:D11 B10:E10 B7:C9 E7:E9">
-    <cfRule type="containsText" dxfId="16" priority="1" stopIfTrue="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1618,20 +1566,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1655,10 +1603,10 @@
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1686,7 +1634,7 @@
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1706,10 +1654,10 @@
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1723,10 +1671,10 @@
       <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1757,7 +1705,7 @@
       <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1771,10 +1719,10 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:C3 B4:E4 B8:E8 B5 D5:E5 B9:C9 E9 B6:C7">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>